<commit_message>
Added register page step def ,feature file and page object
</commit_message>
<xml_diff>
--- a/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
+++ b/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="pythonCode" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="registerData" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -32,31 +33,22 @@
     <t xml:space="preserve">expectedmessage</t>
   </si>
   <si>
-    <t xml:space="preserve">Numpysdet146</t>
+    <t xml:space="preserve">sonali</t>
   </si>
   <si>
     <t xml:space="preserve">user</t>
   </si>
   <si>
-    <t xml:space="preserve">Please check your password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdet146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please check your user id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You are logged in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numpysdet</t>
+    <t xml:space="preserve">Invalid Username and Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dsalgo@1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N2324435</t>
   </si>
   <si>
     <t xml:space="preserve">sdetbatch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid Username and Password</t>
   </si>
   <si>
     <t xml:space="preserve">pythonCode</t>
@@ -145,6 +137,15 @@
   </si>
   <si>
     <t xml:space="preserve">[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmpassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sdet147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demo1234</t>
   </si>
 </sst>
 </file>
@@ -273,10 +274,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -299,7 +300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -310,7 +311,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -318,31 +319,34 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -361,7 +365,7 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -374,90 +378,90 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -469,4 +473,56 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sign in and register feature completed
</commit_message>
<xml_diff>
--- a/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
+++ b/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
     <t xml:space="preserve">expectedmessage</t>
   </si>
   <si>
-    <t xml:space="preserve">sonali</t>
+    <t xml:space="preserve">sdetwarriors</t>
   </si>
   <si>
     <t xml:space="preserve">user</t>
@@ -42,10 +42,10 @@
     <t xml:space="preserve">Invalid Username and Password</t>
   </si>
   <si>
-    <t xml:space="preserve">Dsalgo@1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2324435</t>
+    <t xml:space="preserve">sdet@146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2324435</t>
   </si>
   <si>
     <t xml:space="preserve">sdetbatch</t>
@@ -54,10 +54,10 @@
     <t xml:space="preserve">pythonCode</t>
   </si>
   <si>
-    <t xml:space="preserve">Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">print("hello");</t>
+    <t xml:space="preserve">result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print("hello")</t>
   </si>
   <si>
     <t xml:space="preserve">hello</t>
@@ -277,7 +277,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -348,6 +348,9 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="sdet@146"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -365,8 +368,8 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -482,7 +485,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added stack , queue , and dataStruIntro page and picocontainer
</commit_message>
<xml_diff>
--- a/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
+++ b/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="loginData" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="pythonCode" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="registerData" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="pythonCode_2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="loginData" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="pythonCode" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="registerData" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,34 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
-  <si>
-    <t xml:space="preserve">username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expectedmessage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdetwarriors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid Username and Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdet@146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n2324435</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdetbatch</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t xml:space="preserve">pythonCode</t>
   </si>
@@ -139,13 +113,40 @@
     <t xml:space="preserve">[4, 9, 9, 49, 121]</t>
   </si>
   <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectedmessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdetwarriors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid Username and Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdet@146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2324435</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdetbatch</t>
+  </si>
+  <si>
     <t xml:space="preserve">confirmpassword</t>
   </si>
   <si>
-    <t xml:space="preserve">Sdet147</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demo1234</t>
+    <t xml:space="preserve">Sdet151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demo12345</t>
   </si>
 </sst>
 </file>
@@ -274,6 +275,118 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -291,46 +404,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -361,15 +474,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -381,92 +494,59 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -478,15 +558,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -499,10 +579,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
added allure report with failed case screenshot and arrays page
</commit_message>
<xml_diff>
--- a/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
+++ b/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="pythonCode_2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="pythonCodeSubmission" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="loginData" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="pythonCode" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="registerData" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="pythonArrayQuestion" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t xml:space="preserve">pythonCode</t>
   </si>
@@ -31,10 +32,7 @@
     <t xml:space="preserve">result</t>
   </si>
   <si>
-    <t xml:space="preserve">print("hello")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hello</t>
+    <t xml:space="preserve">actual</t>
   </si>
   <si>
     <t xml:space="preserve">def search(input_list, num):
@@ -51,10 +49,27 @@
 search([12, 23, 45, 67, 6, 90] , 12)</t>
   </si>
   <si>
-    <t xml:space="preserve">Element Found</t>
-  </si>
-  <si>
     <t xml:space="preserve">submission success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some Tests failed. Please review code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def search(input_list, num)
+if(num in input_list)
+print("Element Found")
+\b
+\b
+else:
+print("Not Found")
+\b
+\b
+\b
+\b
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error occurred during submission</t>
   </si>
   <si>
     <t xml:space="preserve">def findMaxConsecutiveOnes(nums) :
@@ -78,7 +93,25 @@
 findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
+    <t xml:space="preserve">def findMaxConsecutiveOnes(nums) 
+count = 0
+result = 0
+for i in range(0, len(nums))
+if (nums[i] == 0)
+count = 0
+\b
+\b
+Else
+count+= 1
+\b
+\b
+result = max(result, count)
+\b
+\b
+print(result)
+\b
+\b
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
   </si>
   <si>
     <t xml:space="preserve">def findNumbers(nums):
@@ -97,6 +130,77 @@
 findNumbers([12,345,2,6,7896])</t>
   </si>
   <si>
+    <t xml:space="preserve">No tests were collected </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def findNumbers(nums)
+c=0
+for i in nums
+j=str(i)
+x=len(j)
+if x%2==0
+c=c+1
+\b
+\b
+\b
+\b
+print c
+return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def sortedSquares(nums)
+squares_list = []
+for i in range(0, len(nums))
+square = nums[i] * nums[i]
+squares_list.append(square)
+\b
+\b
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list
+return sorted_squares_list
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectedmessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdetwarriors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid Username and Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdet@146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2324435</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdetbatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print("hello")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Element Found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
     <t xml:space="preserve">def sortedSquares(nums):
 squares_list = []
 for i in range(0, len(nums)):
@@ -113,33 +217,6 @@
     <t xml:space="preserve">[4, 9, 9, 49, 121]</t>
   </si>
   <si>
-    <t xml:space="preserve">username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expectedmessage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdetwarriors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid Username and Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdet@146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n2324435</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdetbatch</t>
-  </si>
-  <si>
     <t xml:space="preserve">confirmpassword</t>
   </si>
   <si>
@@ -147,6 +224,42 @@
   </si>
   <si>
     <t xml:space="preserve">demo12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PythonCode for Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def search(input_list, num):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">564 is Number is Not Found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output = 'Number is Not Found'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for x in input_list:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if x == num:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output = 'Number is found'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print(str(num) + ' is '+output)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input_list=[12,23,45,56,67]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num=564</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search(input_list,num)</t>
   </si>
 </sst>
 </file>
@@ -203,7 +316,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -211,6 +324,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -237,7 +357,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,6 +366,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,6 +388,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -275,17 +411,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -295,79 +432,82 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="3" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
+    <row r="7" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -404,60 +544,60 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -501,43 +641,43 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+      <c r="B3" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="B4" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
+      <c r="A6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -565,7 +705,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -579,25 +719,117 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
running all in headless
</commit_message>
<xml_diff>
--- a/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
+++ b/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
@@ -220,7 +220,7 @@
     <t xml:space="preserve">confirmpassword</t>
   </si>
   <si>
-    <t xml:space="preserve">Sdet153</t>
+    <t xml:space="preserve">Sdet154</t>
   </si>
   <si>
     <t xml:space="preserve">demo12345</t>
@@ -706,7 +706,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -763,7 +763,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>

</xml_diff>

<commit_message>
update for crossbrowser testing
</commit_message>
<xml_diff>
--- a/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
+++ b/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
@@ -220,7 +220,7 @@
     <t xml:space="preserve">confirmpassword</t>
   </si>
   <si>
-    <t xml:space="preserve">Sdet156</t>
+    <t xml:space="preserve">Sdet161</t>
   </si>
   <si>
     <t xml:space="preserve">demo12345</t>
@@ -413,8 +413,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -530,7 +530,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -622,7 +622,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,10 +703,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -714,7 +714,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,6 +730,9 @@
       <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">

</xml_diff>

<commit_message>
Updated Hooks and Pom.xml
</commit_message>
<xml_diff>
--- a/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
+++ b/DSAlgoBDDFramework/src/test/resources/TestData/DSAlgoTestData.xlsx
@@ -220,7 +220,7 @@
     <t xml:space="preserve">confirmpassword</t>
   </si>
   <si>
-    <t xml:space="preserve">Sdet161</t>
+    <t xml:space="preserve">Sdet163</t>
   </si>
   <si>
     <t xml:space="preserve">demo12345</t>
@@ -622,7 +622,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -706,7 +706,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>